<commit_message>
during and post MMM weekend
* deprecate .BMMuser json file, user redis for that purpose
* take care with types of BMMuser attributes
* several areascan and raster fixes
* try to get xafs/raster correct in manifest
* explicitly stringify several spreadsheet columns
* when running xafs() with prompt, set BMM.instrument to ''
* begin deprecating analog ROI code
* add to Fe standards spreadsheet
</commit_message>
<xml_diff>
--- a/startup/standards/Fe.xlsx
+++ b/startup/standards/Fe.xlsx
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="139">
   <si>
     <t xml:space="preserve">Double wheel</t>
   </si>
@@ -425,6 +425,96 @@
   </si>
   <si>
     <t xml:space="preserve">Fe2(C2O4)3(H2O)6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hedenbergite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CaFeSi2O6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andradite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ca3Fe2Si3O12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ilvaite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CaFe(2+)2Fe(3+)(Si2O7)OOH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epidote</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ca2Al2Fe(SiO4)(Si2O7)OOH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hornblende</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ca2Fe4Al0.75(Si7AlO22)OH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Almandine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fe3Al2Si3O12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ferro-Axinite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ca2FeAl2BSi4O15OH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Augite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Ca,Na)(Mg,Fe,Ti,Al)(Si,Al)2O6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chondrodite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Mg,Fe)5(SiO)2(F,OH,O)2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cordierite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Mg,Fe)2Al3(Si5AlO18)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diadochite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fe2(PO4)(SO4)OH.5H2O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ludwigite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mg2FeBO5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neotocite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Mn,Fe,Mg)SiO3.H2O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scozalite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Fe,Mg)Al2(OH,PO4)2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vesuvianite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ca10(Mg,Fe)Al4(Si2O7)2(SiO4)4(OH)4</t>
   </si>
   <si>
     <t xml:space="preserve">Current</t>
@@ -1114,9 +1204,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>93960</xdr:colOff>
+      <xdr:colOff>93600</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>141480</xdr:rowOff>
+      <xdr:rowOff>141120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1125,8 +1215,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3356280" y="10725120"/>
-          <a:ext cx="6648120" cy="2259000"/>
+          <a:off x="3357000" y="10725120"/>
+          <a:ext cx="6648120" cy="2258640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1373,9 +1463,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1098000</xdr:colOff>
+      <xdr:colOff>1097640</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>50400</xdr:rowOff>
+      <xdr:rowOff>50040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1388,8 +1478,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1299600" y="10772280"/>
-          <a:ext cx="1833480" cy="2445840"/>
+          <a:off x="1300320" y="10772280"/>
+          <a:ext cx="1833120" cy="2445480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1415,9 +1505,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>93960</xdr:colOff>
+      <xdr:colOff>93600</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>141480</xdr:rowOff>
+      <xdr:rowOff>141120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1426,8 +1516,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3356280" y="10725120"/>
-          <a:ext cx="6648120" cy="2259000"/>
+          <a:off x="3357000" y="10725120"/>
+          <a:ext cx="6648120" cy="2258640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1674,9 +1764,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1098000</xdr:colOff>
+      <xdr:colOff>1097640</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>50400</xdr:rowOff>
+      <xdr:rowOff>50040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1689,8 +1779,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1299600" y="10772280"/>
-          <a:ext cx="1833480" cy="2445840"/>
+          <a:off x="1300320" y="10772280"/>
+          <a:ext cx="1833120" cy="2445480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1717,10 +1807,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="P1" activeCellId="0" sqref="P1"/>
       <selection pane="bottomLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
-      <selection pane="bottomRight" activeCell="AE1" activeCellId="1" sqref="O7:Q7 AE1"/>
+      <selection pane="bottomRight" activeCell="AE1" activeCellId="0" sqref="AE1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -3738,10 +3828,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="O1" activeCellId="0" sqref="O1"/>
       <selection pane="bottomLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
-      <selection pane="bottomRight" activeCell="AE1" activeCellId="1" sqref="O7:Q7 AE1"/>
+      <selection pane="bottomRight" activeCell="AE1" activeCellId="0" sqref="AE1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -5755,14 +5845,14 @@
   <dimension ref="B1:AD54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="F13" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="O7" activeCellId="0" sqref="O7:Q7"/>
+      <selection pane="bottomLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="E46" activeCellId="0" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -5772,7 +5862,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="29.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="35.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="29.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="41.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="0" width="22.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="18" style="0" width="14.43"/>
@@ -7046,7 +7137,7 @@
       <c r="AA31" s="59"/>
       <c r="AB31" s="60"/>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="48" t="n">
         <v>2</v>
       </c>
@@ -7056,16 +7147,24 @@
       <c r="D32" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="51"/>
+      <c r="E32" s="51" t="s">
+        <v>98</v>
+      </c>
       <c r="F32" s="12"/>
       <c r="G32" s="12"/>
       <c r="H32" s="12"/>
       <c r="I32" s="52"/>
       <c r="J32" s="53"/>
       <c r="K32" s="48"/>
-      <c r="L32" s="54"/>
-      <c r="M32" s="51"/>
-      <c r="N32" s="55"/>
+      <c r="L32" s="54" t="s">
+        <v>99</v>
+      </c>
+      <c r="M32" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="N32" s="55" t="s">
+        <v>79</v>
+      </c>
       <c r="O32" s="54"/>
       <c r="P32" s="29"/>
       <c r="Q32" s="55"/>
@@ -7079,7 +7178,7 @@
       <c r="AA32" s="59"/>
       <c r="AB32" s="60"/>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="48" t="n">
         <v>3</v>
       </c>
@@ -7089,16 +7188,24 @@
       <c r="D33" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E33" s="29"/>
+      <c r="E33" s="29" t="s">
+        <v>100</v>
+      </c>
       <c r="F33" s="12"/>
       <c r="G33" s="12"/>
       <c r="H33" s="12"/>
       <c r="I33" s="52"/>
       <c r="J33" s="53"/>
       <c r="K33" s="48"/>
-      <c r="L33" s="54"/>
-      <c r="M33" s="51"/>
-      <c r="N33" s="55"/>
+      <c r="L33" s="54" t="s">
+        <v>101</v>
+      </c>
+      <c r="M33" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="N33" s="55" t="s">
+        <v>79</v>
+      </c>
       <c r="O33" s="54"/>
       <c r="P33" s="29"/>
       <c r="Q33" s="55"/>
@@ -7112,7 +7219,7 @@
       <c r="AA33" s="59"/>
       <c r="AB33" s="60"/>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="48" t="n">
         <v>4</v>
       </c>
@@ -7122,16 +7229,24 @@
       <c r="D34" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E34" s="29"/>
+      <c r="E34" s="29" t="s">
+        <v>102</v>
+      </c>
       <c r="F34" s="12"/>
       <c r="G34" s="12"/>
       <c r="H34" s="12"/>
       <c r="I34" s="52"/>
       <c r="J34" s="53"/>
       <c r="K34" s="48"/>
-      <c r="L34" s="54"/>
-      <c r="M34" s="51"/>
-      <c r="N34" s="55"/>
+      <c r="L34" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="M34" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="N34" s="55" t="s">
+        <v>79</v>
+      </c>
       <c r="O34" s="54"/>
       <c r="P34" s="29"/>
       <c r="Q34" s="55"/>
@@ -7145,7 +7260,7 @@
       <c r="AA34" s="59"/>
       <c r="AB34" s="60"/>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="48" t="n">
         <v>5</v>
       </c>
@@ -7155,16 +7270,24 @@
       <c r="D35" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E35" s="29"/>
+      <c r="E35" s="29" t="s">
+        <v>104</v>
+      </c>
       <c r="F35" s="12"/>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
       <c r="I35" s="52"/>
       <c r="J35" s="53"/>
       <c r="K35" s="48"/>
-      <c r="L35" s="54"/>
-      <c r="M35" s="51"/>
-      <c r="N35" s="55"/>
+      <c r="L35" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="M35" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="N35" s="55" t="s">
+        <v>79</v>
+      </c>
       <c r="O35" s="54"/>
       <c r="P35" s="29"/>
       <c r="Q35" s="55"/>
@@ -7178,7 +7301,7 @@
       <c r="AA35" s="59"/>
       <c r="AB35" s="60"/>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="48" t="n">
         <v>6</v>
       </c>
@@ -7188,16 +7311,24 @@
       <c r="D36" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E36" s="29"/>
+      <c r="E36" s="29" t="s">
+        <v>106</v>
+      </c>
       <c r="F36" s="12"/>
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
       <c r="I36" s="52"/>
       <c r="J36" s="53"/>
       <c r="K36" s="48"/>
-      <c r="L36" s="54"/>
-      <c r="M36" s="51"/>
-      <c r="N36" s="55"/>
+      <c r="L36" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="M36" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="N36" s="55" t="s">
+        <v>79</v>
+      </c>
       <c r="O36" s="54"/>
       <c r="P36" s="29"/>
       <c r="Q36" s="55"/>
@@ -7211,7 +7342,7 @@
       <c r="AA36" s="59"/>
       <c r="AB36" s="60"/>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="48" t="n">
         <v>7</v>
       </c>
@@ -7221,16 +7352,24 @@
       <c r="D37" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E37" s="29"/>
+      <c r="E37" s="29" t="s">
+        <v>108</v>
+      </c>
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
       <c r="I37" s="52"/>
       <c r="J37" s="53"/>
       <c r="K37" s="48"/>
-      <c r="L37" s="54"/>
-      <c r="M37" s="51"/>
-      <c r="N37" s="55"/>
+      <c r="L37" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="M37" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="N37" s="55" t="s">
+        <v>79</v>
+      </c>
       <c r="O37" s="54"/>
       <c r="P37" s="29"/>
       <c r="Q37" s="55"/>
@@ -7254,16 +7393,24 @@
       <c r="D38" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E38" s="29"/>
+      <c r="E38" s="0" t="s">
+        <v>110</v>
+      </c>
       <c r="F38" s="12"/>
       <c r="G38" s="12"/>
       <c r="H38" s="12"/>
       <c r="I38" s="52"/>
       <c r="J38" s="53"/>
       <c r="K38" s="48"/>
-      <c r="L38" s="54"/>
-      <c r="M38" s="51"/>
-      <c r="N38" s="55"/>
+      <c r="L38" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="M38" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="N38" s="55" t="s">
+        <v>79</v>
+      </c>
       <c r="O38" s="54"/>
       <c r="P38" s="29"/>
       <c r="Q38" s="55"/>
@@ -7277,7 +7424,7 @@
       <c r="AA38" s="59"/>
       <c r="AB38" s="60"/>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="48" t="n">
         <v>9</v>
       </c>
@@ -7287,16 +7434,24 @@
       <c r="D39" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E39" s="29"/>
+      <c r="E39" s="29" t="s">
+        <v>112</v>
+      </c>
       <c r="F39" s="12"/>
       <c r="G39" s="12"/>
       <c r="H39" s="12"/>
       <c r="I39" s="52"/>
       <c r="J39" s="53"/>
       <c r="K39" s="48"/>
-      <c r="L39" s="54"/>
-      <c r="M39" s="51"/>
-      <c r="N39" s="55"/>
+      <c r="L39" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="M39" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="N39" s="55" t="s">
+        <v>79</v>
+      </c>
       <c r="O39" s="54"/>
       <c r="P39" s="29"/>
       <c r="Q39" s="55"/>
@@ -7310,7 +7465,7 @@
       <c r="AA39" s="59"/>
       <c r="AB39" s="60"/>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="48" t="n">
         <v>10</v>
       </c>
@@ -7320,16 +7475,24 @@
       <c r="D40" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E40" s="29"/>
+      <c r="E40" s="29" t="s">
+        <v>114</v>
+      </c>
       <c r="F40" s="12"/>
       <c r="G40" s="12"/>
       <c r="H40" s="12"/>
       <c r="I40" s="52"/>
       <c r="J40" s="53"/>
       <c r="K40" s="48"/>
-      <c r="L40" s="54"/>
-      <c r="M40" s="51"/>
-      <c r="N40" s="55"/>
+      <c r="L40" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="M40" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="N40" s="55" t="s">
+        <v>79</v>
+      </c>
       <c r="O40" s="54"/>
       <c r="P40" s="29"/>
       <c r="Q40" s="55"/>
@@ -7343,7 +7506,7 @@
       <c r="AA40" s="59"/>
       <c r="AB40" s="60"/>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="48" t="n">
         <v>11</v>
       </c>
@@ -7353,16 +7516,24 @@
       <c r="D41" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E41" s="29"/>
+      <c r="E41" s="29" t="s">
+        <v>116</v>
+      </c>
       <c r="F41" s="12"/>
       <c r="G41" s="12"/>
       <c r="H41" s="12"/>
       <c r="I41" s="52"/>
       <c r="J41" s="53"/>
       <c r="K41" s="48"/>
-      <c r="L41" s="54"/>
-      <c r="M41" s="51"/>
-      <c r="N41" s="55"/>
+      <c r="L41" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="M41" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="N41" s="55" t="s">
+        <v>79</v>
+      </c>
       <c r="O41" s="54"/>
       <c r="P41" s="29"/>
       <c r="Q41" s="55"/>
@@ -7376,7 +7547,7 @@
       <c r="AA41" s="59"/>
       <c r="AB41" s="60"/>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="48" t="n">
         <v>12</v>
       </c>
@@ -7386,16 +7557,24 @@
       <c r="D42" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E42" s="29"/>
+      <c r="E42" s="0" t="s">
+        <v>118</v>
+      </c>
       <c r="F42" s="12"/>
       <c r="G42" s="12"/>
       <c r="H42" s="12"/>
       <c r="I42" s="52"/>
       <c r="J42" s="53"/>
       <c r="K42" s="48"/>
-      <c r="L42" s="54"/>
-      <c r="M42" s="51"/>
-      <c r="N42" s="55"/>
+      <c r="L42" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="M42" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="N42" s="55" t="s">
+        <v>79</v>
+      </c>
       <c r="O42" s="54"/>
       <c r="P42" s="29"/>
       <c r="Q42" s="55"/>
@@ -7409,7 +7588,7 @@
       <c r="AA42" s="59"/>
       <c r="AB42" s="60"/>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="48" t="n">
         <v>13</v>
       </c>
@@ -7419,16 +7598,24 @@
       <c r="D43" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E43" s="29"/>
+      <c r="E43" s="29" t="s">
+        <v>120</v>
+      </c>
       <c r="F43" s="12"/>
       <c r="G43" s="12"/>
       <c r="H43" s="12"/>
       <c r="I43" s="52"/>
       <c r="J43" s="53"/>
       <c r="K43" s="48"/>
-      <c r="L43" s="54"/>
-      <c r="M43" s="51"/>
-      <c r="N43" s="55"/>
+      <c r="L43" s="54" t="s">
+        <v>121</v>
+      </c>
+      <c r="M43" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="N43" s="55" t="s">
+        <v>79</v>
+      </c>
       <c r="O43" s="54"/>
       <c r="P43" s="29"/>
       <c r="Q43" s="55"/>
@@ -7442,7 +7629,7 @@
       <c r="AA43" s="59"/>
       <c r="AB43" s="60"/>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="48" t="n">
         <v>14</v>
       </c>
@@ -7452,16 +7639,24 @@
       <c r="D44" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E44" s="29"/>
+      <c r="E44" s="29" t="s">
+        <v>122</v>
+      </c>
       <c r="F44" s="12"/>
       <c r="G44" s="12"/>
       <c r="H44" s="12"/>
       <c r="I44" s="52"/>
       <c r="J44" s="53"/>
       <c r="K44" s="48"/>
-      <c r="L44" s="54"/>
-      <c r="M44" s="51"/>
-      <c r="N44" s="55"/>
+      <c r="L44" s="54" t="s">
+        <v>123</v>
+      </c>
+      <c r="M44" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="N44" s="55" t="s">
+        <v>79</v>
+      </c>
       <c r="O44" s="54"/>
       <c r="P44" s="29"/>
       <c r="Q44" s="55"/>
@@ -7475,7 +7670,7 @@
       <c r="AA44" s="59"/>
       <c r="AB44" s="60"/>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="48" t="n">
         <v>15</v>
       </c>
@@ -7485,16 +7680,24 @@
       <c r="D45" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E45" s="29"/>
+      <c r="E45" s="29" t="s">
+        <v>124</v>
+      </c>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
       <c r="H45" s="12"/>
       <c r="I45" s="52"/>
       <c r="J45" s="53"/>
       <c r="K45" s="48"/>
-      <c r="L45" s="54"/>
-      <c r="M45" s="51"/>
-      <c r="N45" s="55"/>
+      <c r="L45" s="54" t="s">
+        <v>125</v>
+      </c>
+      <c r="M45" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="N45" s="55" t="s">
+        <v>79</v>
+      </c>
       <c r="O45" s="54"/>
       <c r="P45" s="29"/>
       <c r="Q45" s="55"/>
@@ -7772,7 +7975,7 @@
       <c r="AA53" s="59"/>
       <c r="AB53" s="60"/>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="48" t="n">
         <v>24</v>
       </c>
@@ -7782,16 +7985,24 @@
       <c r="D54" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E54" s="29"/>
+      <c r="E54" s="29" t="s">
+        <v>126</v>
+      </c>
       <c r="F54" s="12"/>
       <c r="G54" s="12"/>
       <c r="H54" s="12"/>
       <c r="I54" s="52"/>
       <c r="J54" s="53"/>
       <c r="K54" s="48"/>
-      <c r="L54" s="54"/>
-      <c r="M54" s="29"/>
-      <c r="N54" s="55"/>
+      <c r="L54" s="54" t="s">
+        <v>127</v>
+      </c>
+      <c r="M54" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="N54" s="55" t="s">
+        <v>79</v>
+      </c>
       <c r="O54" s="54"/>
       <c r="P54" s="29"/>
       <c r="Q54" s="55"/>
@@ -7902,10 +8113,10 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="O7:Q7 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>
@@ -7913,12 +8124,12 @@
   <sheetData>
     <row r="1" s="61" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="28" t="s">
-        <v>99</v>
+        <v>129</v>
       </c>
       <c r="B2" s="61"/>
     </row>
@@ -7934,10 +8145,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="28" t="s">
-        <v>99</v>
+        <v>129</v>
       </c>
       <c r="B5" s="61" t="s">
-        <v>100</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7945,7 +8156,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>101</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7953,7 +8164,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>102</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7961,7 +8172,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7969,7 +8180,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7977,7 +8188,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>105</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7985,7 +8196,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>106</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7993,7 +8204,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>107</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8001,7 +8212,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>